<commit_message>
Update SCD0264, SCD0271, SCD0277 (06-20 Oktober) and Scripting SCD0338-001 until SCD0338-007 (21-22 Oktober)
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0264 - Searching profiling nasabah & memiliki sales kelolaan.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0264 - Searching profiling nasabah & memiliki sales kelolaan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674E0FD9-B44A-4D61-84BE-CEE36AC5FC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BA9DF9-B72D-4C73-AD7D-351C24A23FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>RUN</t>
   </si>
@@ -199,9 +199,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -216,10 +215,28 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,13 +545,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.85546875" customWidth="1"/>
     <col min="4" max="4" width="62.42578125" bestFit="1" customWidth="1"/>
@@ -557,288 +572,289 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="229.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="9">
         <v>23320</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="9">
         <v>9938132562</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="12" t="s">
         <v>16</v>
       </c>
       <c r="O2" s="9">
         <v>9448808661</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
     </row>
     <row r="3" spans="1:20" ht="229.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="9">
         <v>20478</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="2"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:20" ht="229.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="9">
         <v>23320</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="I4" s="8"/>
+      <c r="J4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="M4" s="9">
         <v>9938132562</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="12" t="s">
         <v>16</v>
       </c>
       <c r="O4" s="9">
         <v>9448808661</v>
       </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="2"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:20" ht="229.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="9">
         <v>19264</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
       <c r="M5" s="9"/>
-      <c r="N5" s="7"/>
+      <c r="N5" s="12"/>
       <c r="O5" s="9"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="2"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:20" ht="229.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="9">
         <v>23320</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4" t="s">
+      <c r="I6" s="8"/>
+      <c r="J6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="8" t="s">
         <v>23</v>
       </c>
       <c r="M6" s="9">
         <v>9938132562</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="12" t="s">
         <v>16</v>
       </c>
       <c r="O6" s="9">
         <v>9448808661</v>
       </c>
-      <c r="P6" s="8"/>
+      <c r="P6" s="13"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="9"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>